<commit_message>
Ajuste do nome da coluna
</commit_message>
<xml_diff>
--- a/SME.ConectaFormacao.Webapi/Modelos/planilha_inscricao_cursista.xlsx
+++ b/SME.ConectaFormacao.Webapi/Modelos/planilha_inscricao_cursista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\SME-Conecta-Formacao\SME.ConectaFormacao.Webapi\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8CA55D-A612-40C0-B043-1DD04322B32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6061EED-B81A-4BDD-A0F3-AE7F2686A769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FECD54D1-8E71-4471-8C2F-8A4D27FEDEA6}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>NOME</t>
   </si>
   <si>
-    <t>TURMA1</t>
+    <t>TURMA</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>